<commit_message>
Aggiunto due cosine all'excel che potrebbero facilitare l'inserimento dei dati
</commit_message>
<xml_diff>
--- a/Data/MichelsonNico.xlsx
+++ b/Data/MichelsonNico.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17426"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicoc_000\Desktop\Università\Laboratorio di fisica\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\passa\Documents\Scuola\Corsi\Fisica\Laboratorio\LaboratorioOtticaElettronicaFModerna\Git\InterferometroMichelson\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5664" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="5670" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Lunghezza d'onda" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>delta x</t>
   </si>
@@ -72,6 +72,18 @@
   </si>
   <si>
     <t>lambda media ^2</t>
+  </si>
+  <si>
+    <t>Misura</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Misura </t>
+  </si>
+  <si>
+    <t>Errore</t>
+  </si>
+  <si>
+    <t>Errore delta x</t>
   </si>
 </sst>
 </file>
@@ -111,7 +123,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -127,7 +139,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -423,51 +435,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:B22"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2">
+        <f>A2/5</f>
+        <v>0</v>
+      </c>
+      <c r="C2">
         <v>10</v>
       </c>
-      <c r="C2">
-        <f>2*$B$21*A2/B2</f>
+      <c r="D2">
+        <f>2*$B$21*B2/C2</f>
         <v>0</v>
       </c>
-      <c r="D2">
-        <f>(2*$B$21*$B$22/B2)</f>
+      <c r="E2">
+        <f>(2*$B$21*$B$22/C2)</f>
         <v>2.0005852000000001E-7</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>1</v>
       </c>
@@ -475,7 +494,7 @@
         <v>1.0002926000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>5</v>
       </c>
@@ -494,15 +513,15 @@
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -510,18 +529,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B2" t="e">
         <f>A2*B23/(2*B24)+1</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>1</v>
       </c>
@@ -529,7 +548,7 @@
         <v>1.0002926000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>5</v>
       </c>
@@ -538,12 +557,12 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -558,10 +577,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -569,41 +588,56 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C2" t="e">
-        <f>B2*B24/(2*A2)</f>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <f>A2/5</f>
+        <v>0</v>
+      </c>
+      <c r="D2" t="e">
+        <f>C2*B24/(2*B2)</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="E2" t="e">
+        <f>D2/B2*B25</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -612,7 +646,7 @@
         <v>5.8899999999999999E-7</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>10</v>
       </c>
@@ -621,7 +655,7 @@
         <v>5.8960000000000004E-7</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -630,13 +664,22 @@
         <v>5.8930000000000002E-7</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>14</v>
       </c>
       <c r="B24">
         <f>B23^2</f>
         <v>3.4727449000000003E-13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25">
+        <f>'Lunghezza d''onda'!B22</f>
+        <v>9.9999999999999995E-7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>